<commit_message>
made a publish and changed the excel sample files
</commit_message>
<xml_diff>
--- a/_Sample_ExcelFiles/fileA.xlsx
+++ b/_Sample_ExcelFiles/fileA.xlsx
@@ -1,26 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\1VlookupTestFiles\ExcelTestFile\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cipri\github\CSharp_VLookupTool\_Sample_ExcelFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1BE70DD8-5941-4F7C-9215-885023507BEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{73B4EEAC-0B80-4D75-901F-5944395595CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3690" yWindow="1125" windowWidth="38700" windowHeight="15345" tabRatio="205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3900" yWindow="3900" windowWidth="38700" windowHeight="15345" xr2:uid="{1DA1308E-32BD-4160-AAB5-C39B7F83858D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+      <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>First Name</t>
   </si>
@@ -28,78 +44,110 @@
     <t>Last Name</t>
   </si>
   <si>
-    <t>Id</t>
-  </si>
-  <si>
-    <t>Dulce</t>
-  </si>
-  <si>
-    <t>Abril</t>
-  </si>
-  <si>
-    <t>Mara</t>
-  </si>
-  <si>
-    <t>Hashimoto</t>
-  </si>
-  <si>
-    <t>Philip</t>
-  </si>
-  <si>
-    <t>Gent</t>
-  </si>
-  <si>
-    <t>Kathleen</t>
-  </si>
-  <si>
-    <t>Hanner</t>
-  </si>
-  <si>
-    <t>Nereida</t>
-  </si>
-  <si>
-    <t>Magwood</t>
-  </si>
-  <si>
-    <t>Gaston</t>
-  </si>
-  <si>
-    <t>Brumm</t>
-  </si>
-  <si>
-    <t>Etta</t>
-  </si>
-  <si>
-    <t>Hurn</t>
-  </si>
-  <si>
-    <t>Earlean</t>
-  </si>
-  <si>
-    <t>Melgar</t>
-  </si>
-  <si>
-    <t>Vincenza</t>
-  </si>
-  <si>
-    <t>Weiland</t>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Alice</t>
+  </si>
+  <si>
+    <t>Smith</t>
+  </si>
+  <si>
+    <t>Bob</t>
+  </si>
+  <si>
+    <t>Jones</t>
+  </si>
+  <si>
+    <t>Charlie</t>
+  </si>
+  <si>
+    <t>Brown</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Lee</t>
+  </si>
+  <si>
+    <t>Eve</t>
+  </si>
+  <si>
+    <t>Green</t>
+  </si>
+  <si>
+    <t>Frank</t>
+  </si>
+  <si>
+    <t>White</t>
+  </si>
+  <si>
+    <t>Grace</t>
+  </si>
+  <si>
+    <t>Chen</t>
+  </si>
+  <si>
+    <t>Harry</t>
+  </si>
+  <si>
+    <t>Potter</t>
+  </si>
+  <si>
+    <t>Irene</t>
+  </si>
+  <si>
+    <t>Kim</t>
+  </si>
+  <si>
+    <t>Jack</t>
+  </si>
+  <si>
+    <t>Black</t>
+  </si>
+  <si>
+    <t>Kate</t>
+  </si>
+  <si>
+    <t>Wilson</t>
+  </si>
+  <si>
+    <t>Leo</t>
+  </si>
+  <si>
+    <t>Garcia</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Nick</t>
+  </si>
+  <si>
+    <t>Miller</t>
+  </si>
+  <si>
+    <t>Olivia</t>
+  </si>
+  <si>
+    <t>Taylor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -122,9 +170,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -438,132 +485,196 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE54D9F2-AC37-40D4-A40D-76822B4EC817}">
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1020" width="11.5703125"/>
+    <col min="1" max="1" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1234567890</v>
+      </c>
+      <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>4</v>
       </c>
-      <c r="C2">
-        <v>1562</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2345678901</v>
+      </c>
+      <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="C3">
-        <v>1582</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3456789012</v>
+      </c>
+      <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="C4">
-        <v>2587</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4567890123</v>
+      </c>
+      <c r="B5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5" t="s">
         <v>10</v>
       </c>
-      <c r="C5">
-        <v>3549</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5678901234</v>
+      </c>
+      <c r="B6" t="s">
         <v>11</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>12</v>
       </c>
-      <c r="C6">
-        <v>2468</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6789012345</v>
+      </c>
+      <c r="B7" t="s">
         <v>13</v>
       </c>
-      <c r="B7" t="s">
+      <c r="C7" t="s">
         <v>14</v>
       </c>
-      <c r="C7">
-        <v>2554</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7890123456</v>
+      </c>
+      <c r="B8" t="s">
         <v>15</v>
       </c>
-      <c r="B8" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="C8">
-        <v>3598</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8901234567</v>
+      </c>
+      <c r="B9" t="s">
         <v>17</v>
       </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>18</v>
       </c>
-      <c r="C9">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9012345678</v>
+      </c>
+      <c r="B10" t="s">
         <v>19</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>20</v>
       </c>
-      <c r="C10">
-        <v>6548</v>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>123456789</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>987654321</v>
+      </c>
+      <c r="B12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>9876543210</v>
+      </c>
+      <c r="B13" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>8765432109</v>
+      </c>
+      <c r="B14" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>7654321098</v>
+      </c>
+      <c r="B15" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>6543210987</v>
+      </c>
+      <c r="B16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
-  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
-  <headerFooter>
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>